<commit_message>
Updating Scenathon data + SOFA alternative pathways
Updating Scenathon figures on GHG and Scenarios assumptions with new database + SOFA alternative pathways (GS_crop etc.) extracing values about food waste and crop/live prod.ty for Steven
</commit_message>
<xml_diff>
--- a/data/mapping_alpha3_Country.xlsx
+++ b/data/mapping_alpha3_Country.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clara Douzal\Documents\Github Desktop\Scenathon2023\data\scenathon_2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Desktop\GitHub\SOFA 2024\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F593E091-80ED-463F-9751-2E376E5CB522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B619C918-AA5A-4054-B478-E0F9597742CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{33C44AA0-F2DD-4818-9A38-8C5D6E240ECA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{33C44AA0-F2DD-4818-9A38-8C5D6E240ECA}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t>ALPHA3</t>
   </si>
@@ -253,9 +253,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -293,7 +293,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -399,7 +399,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -541,7 +541,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -549,15 +549,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E76CDF70-20D0-4966-A8B7-20CFA9C5AC04}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -565,7 +568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -573,7 +576,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -581,7 +584,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -589,7 +592,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -597,7 +600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -605,7 +608,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -613,7 +616,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -621,7 +624,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -629,7 +632,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -637,155 +640,171 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>51</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>22</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>47</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>24</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>28</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>49</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>30</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>46</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>32</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>34</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>35</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>37</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B27" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>39</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>41</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>53</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>43</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>43</v>
       </c>
     </row>
@@ -795,6 +814,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010042E92E7B33C78A4A9E37EE3CE1D07C23" ma:contentTypeVersion="8" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="be478a3e7a78a108573eaae8c7cc1cce">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="66f9c1a9-8286-49e7-922b-17b76842e744" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e534b287ec7ca242b14628634a80063d" ns3:_="">
     <xsd:import namespace="66f9c1a9-8286-49e7-922b-17b76842e744"/>
@@ -966,15 +994,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -982,6 +1001,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1671626C-DAC7-44F8-A95E-69C0720F2086}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EA6DA14-9063-4CBF-8A12-E3BDF6499604}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -995,14 +1022,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1671626C-DAC7-44F8-A95E-69C0720F2086}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>